<commit_message>
Updated headers for consistency
</commit_message>
<xml_diff>
--- a/excel_example.xlsx
+++ b/excel_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricks/Documents/GitHub/python-outlook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCFCC120-7293-8E47-8372-CF1DF0250BCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FACDA5-DC08-5C43-90D2-8EDF9D69FCB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="580" windowWidth="25440" windowHeight="14300" xr2:uid="{E4082F53-782A-404C-BD3D-5715984D15F4}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14300" xr2:uid="{E4082F53-782A-404C-BD3D-5715984D15F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,15 +30,9 @@
     <t>name</t>
   </si>
   <si>
-    <t>header</t>
-  </si>
-  <si>
     <t>message</t>
   </si>
   <si>
-    <t>filepath</t>
-  </si>
-  <si>
     <t>bob@example.com</t>
   </si>
   <si>
@@ -73,6 +67,12 @@
   </si>
   <si>
     <t>C:\reports\food-sales.txt</t>
+  </si>
+  <si>
+    <t>attachment</t>
+  </si>
+  <si>
+    <t>subject</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -444,55 +444,55 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>